<commit_message>
Added EOC data and created key_var_tbl script
</commit_message>
<xml_diff>
--- a/Data/GeoMicro/Micah_EOC/geomicro_EOC_Key_V3.xlsx
+++ b/Data/GeoMicro/Micah_EOC/geomicro_EOC_Key_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\EDaH\Data\GeoMicro\Micah_EOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929A3A37-EAFD-49DF-8871-33AFC94772A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C21C61-B514-4AC2-A0B2-15F634E31D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="3492" windowWidth="30984" windowHeight="12072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Location_data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="661">
   <si>
     <t>var</t>
   </si>
@@ -1996,9 +1996,6 @@
     <t>Extractable organic C</t>
   </si>
   <si>
-    <t>c.per.g.soil</t>
-  </si>
-  <si>
     <t>Specify method for extractable C</t>
   </si>
   <si>
@@ -2009,6 +2006,15 @@
   </si>
   <si>
     <t>eoc_method</t>
+  </si>
+  <si>
+    <t>c_per_g_soil</t>
+  </si>
+  <si>
+    <t>mm-yyyy</t>
+  </si>
+  <si>
+    <t>collection_date</t>
   </si>
 </sst>
 </file>
@@ -2477,23 +2483,23 @@
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6328125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="31.6328125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.08984375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" style="6"/>
-    <col min="6" max="6" width="7.6328125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="38.90625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" style="6" customWidth="1"/>
-    <col min="9" max="14" width="8.90625" style="6"/>
-    <col min="15" max="15" width="12.6328125" style="6"/>
-    <col min="16" max="16" width="16.36328125" style="6" customWidth="1"/>
-    <col min="17" max="16384" width="12.6328125" style="6"/>
+    <col min="1" max="1" width="30.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="6"/>
+    <col min="6" max="6" width="7.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="38.88671875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" style="6" customWidth="1"/>
+    <col min="9" max="14" width="8.88671875" style="6"/>
+    <col min="15" max="15" width="12.6640625" style="6"/>
+    <col min="16" max="16" width="16.33203125" style="6" customWidth="1"/>
+    <col min="17" max="16384" width="12.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>174</v>
       </c>
@@ -2556,7 +2562,7 @@
       <c r="AB1" s="11"/>
       <c r="AC1" s="11"/>
     </row>
-    <row r="2" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>631</v>
       </c>
@@ -2600,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>634</v>
       </c>
@@ -2644,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>635</v>
       </c>
@@ -2688,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>636</v>
       </c>
@@ -2732,7 +2738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -2773,7 +2779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -2814,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>2</v>
       </c>
@@ -2855,7 +2861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>650</v>
       </c>
@@ -2899,7 +2905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>651</v>
       </c>
@@ -2943,7 +2949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
@@ -3025,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>632</v>
       </c>
@@ -3083,7 +3089,7 @@
       <c r="AB13" s="12"/>
       <c r="AC13" s="12"/>
     </row>
-    <row r="14" spans="1:29" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>652</v>
       </c>
@@ -3141,7 +3147,7 @@
       <c r="AB14" s="12"/>
       <c r="AC14" s="12"/>
     </row>
-    <row r="15" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>633</v>
       </c>
@@ -3185,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>1</v>
       </c>
@@ -3229,7 +3235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>2</v>
       </c>
@@ -3270,7 +3276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>2</v>
       </c>
@@ -3883,7 +3889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>575</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C34" s="6" t="s">
         <v>31</v>
       </c>
@@ -3962,7 +3968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>2</v>
       </c>
@@ -4003,7 +4009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C36" s="6" t="s">
         <v>35</v>
       </c>
@@ -4041,7 +4047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C37" s="6" t="s">
         <v>37</v>
       </c>
@@ -5700,7 +5706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
@@ -5709,7 +5715,7 @@
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
     </row>
-    <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
@@ -5718,7 +5724,7 @@
       <c r="G81" s="12"/>
       <c r="H81" s="12"/>
     </row>
-    <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
@@ -5727,7 +5733,7 @@
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
     </row>
-    <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12"/>
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
@@ -5736,7 +5742,7 @@
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
     </row>
-    <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
@@ -5745,7 +5751,7 @@
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
     </row>
-    <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
@@ -5754,7 +5760,7 @@
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
     </row>
-    <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
@@ -5763,7 +5769,7 @@
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
     </row>
-    <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
@@ -5772,7 +5778,7 @@
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
     </row>
-    <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
@@ -5781,7 +5787,7 @@
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
     </row>
-    <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" s="12"/>
       <c r="C89" s="12"/>
@@ -5790,7 +5796,7 @@
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
     </row>
-    <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" s="12"/>
       <c r="C90" s="12"/>
@@ -5799,7 +5805,7 @@
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
     </row>
-    <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" s="12"/>
       <c r="C91" s="12"/>
@@ -5808,7 +5814,7 @@
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
     </row>
-    <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
@@ -5817,7 +5823,7 @@
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
     </row>
-    <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
@@ -5826,7 +5832,7 @@
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
     </row>
-    <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" s="12"/>
       <c r="C94" s="12"/>
@@ -5835,7 +5841,7 @@
       <c r="G94" s="12"/>
       <c r="H94" s="12"/>
     </row>
-    <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" s="12"/>
       <c r="C95" s="12"/>
@@ -5844,7 +5850,7 @@
       <c r="G95" s="12"/>
       <c r="H95" s="12"/>
     </row>
-    <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" s="12"/>
       <c r="C96" s="12"/>
@@ -5853,7 +5859,7 @@
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
     </row>
-    <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" s="12"/>
       <c r="C97" s="12"/>
@@ -5862,7 +5868,7 @@
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
     </row>
-    <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" s="12"/>
       <c r="C98" s="12"/>
@@ -5871,7 +5877,7 @@
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
     </row>
-    <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" s="12"/>
       <c r="C99" s="12"/>
@@ -5880,7 +5886,7 @@
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
     </row>
-    <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" s="12"/>
       <c r="C100" s="12"/>
@@ -5889,7 +5895,7 @@
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
     </row>
-    <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
       <c r="B101" s="12"/>
       <c r="C101" s="12"/>
@@ -5898,7 +5904,7 @@
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
     </row>
-    <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
       <c r="B102" s="12"/>
       <c r="C102" s="12"/>
@@ -5907,7 +5913,7 @@
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
     </row>
-    <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
@@ -5916,7 +5922,7 @@
       <c r="G103" s="12"/>
       <c r="H103" s="12"/>
     </row>
-    <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" s="12"/>
       <c r="C104" s="12"/>
@@ -5925,7 +5931,7 @@
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
     </row>
-    <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" s="12"/>
       <c r="C105" s="12"/>
@@ -5934,7 +5940,7 @@
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
     </row>
-    <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" s="12"/>
       <c r="C106" s="12"/>
@@ -5943,7 +5949,7 @@
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
     </row>
-    <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
@@ -5952,7 +5958,7 @@
       <c r="G107" s="12"/>
       <c r="H107" s="12"/>
     </row>
-    <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="B108" s="12"/>
       <c r="C108" s="12"/>
@@ -5961,7 +5967,7 @@
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
     </row>
-    <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
@@ -5970,7 +5976,7 @@
       <c r="G109" s="12"/>
       <c r="H109" s="12"/>
     </row>
-    <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="B110" s="12"/>
       <c r="C110" s="12"/>
@@ -5979,7 +5985,7 @@
       <c r="G110" s="12"/>
       <c r="H110" s="12"/>
     </row>
-    <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="B111" s="12"/>
       <c r="C111" s="12"/>
@@ -5988,7 +5994,7 @@
       <c r="G111" s="12"/>
       <c r="H111" s="12"/>
     </row>
-    <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
@@ -5997,7 +6003,7 @@
       <c r="G112" s="12"/>
       <c r="H112" s="12"/>
     </row>
-    <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
@@ -6006,7 +6012,7 @@
       <c r="G113" s="12"/>
       <c r="H113" s="12"/>
     </row>
-    <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="12"/>
       <c r="C114" s="12"/>
@@ -6015,7 +6021,7 @@
       <c r="G114" s="12"/>
       <c r="H114" s="12"/>
     </row>
-    <row r="115" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="B115" s="12"/>
       <c r="C115" s="12"/>
@@ -6024,7 +6030,7 @@
       <c r="G115" s="12"/>
       <c r="H115" s="12"/>
     </row>
-    <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="B116" s="12"/>
       <c r="C116" s="12"/>
@@ -6033,7 +6039,7 @@
       <c r="G116" s="12"/>
       <c r="H116" s="12"/>
     </row>
-    <row r="117" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
@@ -6042,7 +6048,7 @@
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
     </row>
-    <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="B118" s="12"/>
       <c r="C118" s="12"/>
@@ -6051,7 +6057,7 @@
       <c r="G118" s="12"/>
       <c r="H118" s="12"/>
     </row>
-    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="B119" s="12"/>
       <c r="C119" s="12"/>
@@ -6060,7 +6066,7 @@
       <c r="G119" s="12"/>
       <c r="H119" s="12"/>
     </row>
-    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="B120" s="12"/>
       <c r="C120" s="12"/>
@@ -6069,7 +6075,7 @@
       <c r="G120" s="12"/>
       <c r="H120" s="12"/>
     </row>
-    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="B121" s="12"/>
       <c r="C121" s="12"/>
@@ -6078,7 +6084,7 @@
       <c r="G121" s="12"/>
       <c r="H121" s="12"/>
     </row>
-    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="B122" s="12"/>
       <c r="C122" s="12"/>
@@ -6087,7 +6093,7 @@
       <c r="G122" s="12"/>
       <c r="H122" s="12"/>
     </row>
-    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="B123" s="12"/>
       <c r="C123" s="12"/>
@@ -6096,7 +6102,7 @@
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
     </row>
-    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="B124" s="12"/>
       <c r="C124" s="12"/>
@@ -6105,7 +6111,7 @@
       <c r="G124" s="12"/>
       <c r="H124" s="12"/>
     </row>
-    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="12"/>
       <c r="C125" s="12"/>
@@ -6114,7 +6120,7 @@
       <c r="G125" s="12"/>
       <c r="H125" s="12"/>
     </row>
-    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
       <c r="B126" s="12"/>
       <c r="C126" s="12"/>
@@ -6123,7 +6129,7 @@
       <c r="G126" s="12"/>
       <c r="H126" s="12"/>
     </row>
-    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12"/>
       <c r="B127" s="12"/>
       <c r="C127" s="12"/>
@@ -6132,7 +6138,7 @@
       <c r="G127" s="12"/>
       <c r="H127" s="12"/>
     </row>
-    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12"/>
       <c r="B128" s="12"/>
       <c r="C128" s="12"/>
@@ -6141,7 +6147,7 @@
       <c r="G128" s="12"/>
       <c r="H128" s="12"/>
     </row>
-    <row r="129" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="B129" s="12"/>
       <c r="C129" s="12"/>
@@ -6150,7 +6156,7 @@
       <c r="G129" s="12"/>
       <c r="H129" s="12"/>
     </row>
-    <row r="130" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="B130" s="12"/>
       <c r="C130" s="12"/>
@@ -6159,7 +6165,7 @@
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
     </row>
-    <row r="131" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="B131" s="12"/>
       <c r="C131" s="12"/>
@@ -6168,7 +6174,7 @@
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
     </row>
-    <row r="132" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="B132" s="12"/>
       <c r="C132" s="12"/>
@@ -6177,7 +6183,7 @@
       <c r="G132" s="12"/>
       <c r="H132" s="12"/>
     </row>
-    <row r="133" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="B133" s="12"/>
       <c r="C133" s="12"/>
@@ -6186,7 +6192,7 @@
       <c r="G133" s="12"/>
       <c r="H133" s="12"/>
     </row>
-    <row r="134" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="B134" s="12"/>
       <c r="C134" s="12"/>
@@ -6195,7 +6201,7 @@
       <c r="G134" s="12"/>
       <c r="H134" s="12"/>
     </row>
-    <row r="135" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="B135" s="12"/>
       <c r="C135" s="12"/>
@@ -6204,7 +6210,7 @@
       <c r="G135" s="12"/>
       <c r="H135" s="12"/>
     </row>
-    <row r="136" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="B136" s="12"/>
       <c r="C136" s="12"/>
@@ -6213,7 +6219,7 @@
       <c r="G136" s="12"/>
       <c r="H136" s="12"/>
     </row>
-    <row r="137" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="B137" s="12"/>
       <c r="C137" s="12"/>
@@ -6222,7 +6228,7 @@
       <c r="G137" s="12"/>
       <c r="H137" s="12"/>
     </row>
-    <row r="138" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="B138" s="12"/>
       <c r="C138" s="12"/>
@@ -6231,7 +6237,7 @@
       <c r="G138" s="12"/>
       <c r="H138" s="12"/>
     </row>
-    <row r="139" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="B139" s="12"/>
       <c r="C139" s="12"/>
@@ -6240,7 +6246,7 @@
       <c r="G139" s="12"/>
       <c r="H139" s="12"/>
     </row>
-    <row r="140" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="B140" s="12"/>
       <c r="C140" s="12"/>
@@ -6249,7 +6255,7 @@
       <c r="G140" s="12"/>
       <c r="H140" s="12"/>
     </row>
-    <row r="141" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
@@ -6258,7 +6264,7 @@
       <c r="G141" s="12"/>
       <c r="H141" s="12"/>
     </row>
-    <row r="142" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="B142" s="12"/>
       <c r="C142" s="12"/>
@@ -6267,7 +6273,7 @@
       <c r="G142" s="12"/>
       <c r="H142" s="12"/>
     </row>
-    <row r="143" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="B143" s="12"/>
       <c r="C143" s="12"/>
@@ -6276,7 +6282,7 @@
       <c r="G143" s="12"/>
       <c r="H143" s="12"/>
     </row>
-    <row r="144" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="B144" s="12"/>
       <c r="C144" s="12"/>
@@ -6285,7 +6291,7 @@
       <c r="G144" s="12"/>
       <c r="H144" s="12"/>
     </row>
-    <row r="145" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="B145" s="12"/>
       <c r="C145" s="12"/>
@@ -6294,7 +6300,7 @@
       <c r="G145" s="12"/>
       <c r="H145" s="12"/>
     </row>
-    <row r="146" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="B146" s="12"/>
       <c r="C146" s="12"/>
@@ -6303,7 +6309,7 @@
       <c r="G146" s="12"/>
       <c r="H146" s="12"/>
     </row>
-    <row r="147" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="B147" s="12"/>
       <c r="C147" s="12"/>
@@ -6312,7 +6318,7 @@
       <c r="G147" s="12"/>
       <c r="H147" s="12"/>
     </row>
-    <row r="148" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="B148" s="12"/>
       <c r="C148" s="12"/>
@@ -6321,7 +6327,7 @@
       <c r="G148" s="12"/>
       <c r="H148" s="12"/>
     </row>
-    <row r="149" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="B149" s="12"/>
       <c r="C149" s="12"/>
@@ -6330,7 +6336,7 @@
       <c r="G149" s="12"/>
       <c r="H149" s="12"/>
     </row>
-    <row r="150" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="B150" s="12"/>
       <c r="C150" s="12"/>
@@ -6339,7 +6345,7 @@
       <c r="G150" s="12"/>
       <c r="H150" s="12"/>
     </row>
-    <row r="151" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
       <c r="B151" s="12"/>
       <c r="C151" s="12"/>
@@ -6348,7 +6354,7 @@
       <c r="G151" s="12"/>
       <c r="H151" s="12"/>
     </row>
-    <row r="152" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
       <c r="B152" s="12"/>
       <c r="C152" s="12"/>
@@ -6357,7 +6363,7 @@
       <c r="G152" s="12"/>
       <c r="H152" s="12"/>
     </row>
-    <row r="153" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12"/>
       <c r="B153" s="12"/>
       <c r="C153" s="12"/>
@@ -6366,7 +6372,7 @@
       <c r="G153" s="12"/>
       <c r="H153" s="12"/>
     </row>
-    <row r="154" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="B154" s="12"/>
       <c r="C154" s="12"/>
@@ -6375,7 +6381,7 @@
       <c r="G154" s="12"/>
       <c r="H154" s="12"/>
     </row>
-    <row r="155" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="B155" s="12"/>
       <c r="C155" s="12"/>
@@ -6384,7 +6390,7 @@
       <c r="G155" s="12"/>
       <c r="H155" s="12"/>
     </row>
-    <row r="156" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="B156" s="12"/>
       <c r="C156" s="12"/>
@@ -6393,7 +6399,7 @@
       <c r="G156" s="12"/>
       <c r="H156" s="12"/>
     </row>
-    <row r="157" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="B157" s="12"/>
       <c r="C157" s="12"/>
@@ -6402,7 +6408,7 @@
       <c r="G157" s="12"/>
       <c r="H157" s="12"/>
     </row>
-    <row r="158" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="B158" s="12"/>
       <c r="C158" s="12"/>
@@ -6411,7 +6417,7 @@
       <c r="G158" s="12"/>
       <c r="H158" s="12"/>
     </row>
-    <row r="159" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="B159" s="12"/>
       <c r="C159" s="12"/>
@@ -6420,7 +6426,7 @@
       <c r="G159" s="12"/>
       <c r="H159" s="12"/>
     </row>
-    <row r="160" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="B160" s="12"/>
       <c r="C160" s="12"/>
@@ -6429,7 +6435,7 @@
       <c r="G160" s="12"/>
       <c r="H160" s="12"/>
     </row>
-    <row r="161" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="B161" s="12"/>
       <c r="C161" s="12"/>
@@ -6438,7 +6444,7 @@
       <c r="G161" s="12"/>
       <c r="H161" s="12"/>
     </row>
-    <row r="162" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="B162" s="12"/>
       <c r="C162" s="12"/>
@@ -6447,7 +6453,7 @@
       <c r="G162" s="12"/>
       <c r="H162" s="12"/>
     </row>
-    <row r="163" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="B163" s="12"/>
       <c r="C163" s="12"/>
@@ -6456,7 +6462,7 @@
       <c r="G163" s="12"/>
       <c r="H163" s="12"/>
     </row>
-    <row r="164" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="B164" s="12"/>
       <c r="C164" s="12"/>
@@ -6465,7 +6471,7 @@
       <c r="G164" s="12"/>
       <c r="H164" s="12"/>
     </row>
-    <row r="165" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="B165" s="12"/>
       <c r="C165" s="12"/>
@@ -6474,7 +6480,7 @@
       <c r="G165" s="12"/>
       <c r="H165" s="12"/>
     </row>
-    <row r="166" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="B166" s="12"/>
       <c r="C166" s="12"/>
@@ -6483,7 +6489,7 @@
       <c r="G166" s="12"/>
       <c r="H166" s="12"/>
     </row>
-    <row r="167" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="B167" s="12"/>
       <c r="C167" s="12"/>
@@ -6492,7 +6498,7 @@
       <c r="G167" s="12"/>
       <c r="H167" s="12"/>
     </row>
-    <row r="168" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="B168" s="12"/>
       <c r="C168" s="12"/>
@@ -6501,7 +6507,7 @@
       <c r="G168" s="12"/>
       <c r="H168" s="12"/>
     </row>
-    <row r="169" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="B169" s="12"/>
       <c r="C169" s="12"/>
@@ -6510,7 +6516,7 @@
       <c r="G169" s="12"/>
       <c r="H169" s="12"/>
     </row>
-    <row r="170" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="B170" s="12"/>
       <c r="C170" s="12"/>
@@ -6519,7 +6525,7 @@
       <c r="G170" s="12"/>
       <c r="H170" s="12"/>
     </row>
-    <row r="171" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="B171" s="12"/>
       <c r="C171" s="12"/>
@@ -6528,7 +6534,7 @@
       <c r="G171" s="12"/>
       <c r="H171" s="12"/>
     </row>
-    <row r="172" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="B172" s="12"/>
       <c r="C172" s="12"/>
@@ -6537,7 +6543,7 @@
       <c r="G172" s="12"/>
       <c r="H172" s="12"/>
     </row>
-    <row r="173" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="B173" s="12"/>
       <c r="C173" s="12"/>
@@ -6546,7 +6552,7 @@
       <c r="G173" s="12"/>
       <c r="H173" s="12"/>
     </row>
-    <row r="174" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="B174" s="12"/>
       <c r="C174" s="12"/>
@@ -6555,7 +6561,7 @@
       <c r="G174" s="12"/>
       <c r="H174" s="12"/>
     </row>
-    <row r="175" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="B175" s="12"/>
       <c r="C175" s="12"/>
@@ -6564,7 +6570,7 @@
       <c r="G175" s="12"/>
       <c r="H175" s="12"/>
     </row>
-    <row r="176" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12"/>
       <c r="B176" s="12"/>
       <c r="C176" s="12"/>
@@ -6573,7 +6579,7 @@
       <c r="G176" s="12"/>
       <c r="H176" s="12"/>
     </row>
-    <row r="177" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="12"/>
       <c r="B177" s="12"/>
       <c r="C177" s="12"/>
@@ -6582,7 +6588,7 @@
       <c r="G177" s="12"/>
       <c r="H177" s="12"/>
     </row>
-    <row r="178" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12"/>
       <c r="B178" s="12"/>
       <c r="C178" s="12"/>
@@ -6591,7 +6597,7 @@
       <c r="G178" s="12"/>
       <c r="H178" s="12"/>
     </row>
-    <row r="179" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" s="12"/>
       <c r="C179" s="12"/>
@@ -6600,7 +6606,7 @@
       <c r="G179" s="12"/>
       <c r="H179" s="12"/>
     </row>
-    <row r="180" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" s="12"/>
       <c r="C180" s="12"/>
@@ -6609,7 +6615,7 @@
       <c r="G180" s="12"/>
       <c r="H180" s="12"/>
     </row>
-    <row r="181" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" s="12"/>
       <c r="C181" s="12"/>
@@ -6618,7 +6624,7 @@
       <c r="G181" s="12"/>
       <c r="H181" s="12"/>
     </row>
-    <row r="182" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="B182" s="12"/>
       <c r="C182" s="12"/>
@@ -6627,7 +6633,7 @@
       <c r="G182" s="12"/>
       <c r="H182" s="12"/>
     </row>
-    <row r="183" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" s="12"/>
       <c r="C183" s="12"/>
@@ -6636,7 +6642,7 @@
       <c r="G183" s="12"/>
       <c r="H183" s="12"/>
     </row>
-    <row r="184" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" s="12"/>
       <c r="C184" s="12"/>
@@ -6645,7 +6651,7 @@
       <c r="G184" s="12"/>
       <c r="H184" s="12"/>
     </row>
-    <row r="185" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="B185" s="12"/>
       <c r="C185" s="12"/>
@@ -6654,7 +6660,7 @@
       <c r="G185" s="12"/>
       <c r="H185" s="12"/>
     </row>
-    <row r="186" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="B186" s="12"/>
       <c r="C186" s="12"/>
@@ -6663,7 +6669,7 @@
       <c r="G186" s="12"/>
       <c r="H186" s="12"/>
     </row>
-    <row r="187" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="B187" s="12"/>
       <c r="C187" s="12"/>
@@ -6672,7 +6678,7 @@
       <c r="G187" s="12"/>
       <c r="H187" s="12"/>
     </row>
-    <row r="188" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="B188" s="12"/>
       <c r="C188" s="12"/>
@@ -6681,7 +6687,7 @@
       <c r="G188" s="12"/>
       <c r="H188" s="12"/>
     </row>
-    <row r="189" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="B189" s="12"/>
       <c r="C189" s="12"/>
@@ -6690,7 +6696,7 @@
       <c r="G189" s="12"/>
       <c r="H189" s="12"/>
     </row>
-    <row r="190" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="B190" s="12"/>
       <c r="C190" s="12"/>
@@ -6699,7 +6705,7 @@
       <c r="G190" s="12"/>
       <c r="H190" s="12"/>
     </row>
-    <row r="191" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="B191" s="12"/>
       <c r="C191" s="12"/>
@@ -6708,7 +6714,7 @@
       <c r="G191" s="12"/>
       <c r="H191" s="12"/>
     </row>
-    <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="B192" s="12"/>
       <c r="C192" s="12"/>
@@ -6717,7 +6723,7 @@
       <c r="G192" s="12"/>
       <c r="H192" s="12"/>
     </row>
-    <row r="193" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="B193" s="12"/>
       <c r="C193" s="12"/>
@@ -6726,7 +6732,7 @@
       <c r="G193" s="12"/>
       <c r="H193" s="12"/>
     </row>
-    <row r="194" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="B194" s="12"/>
       <c r="C194" s="12"/>
@@ -6735,7 +6741,7 @@
       <c r="G194" s="12"/>
       <c r="H194" s="12"/>
     </row>
-    <row r="195" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="B195" s="12"/>
       <c r="C195" s="12"/>
@@ -6744,7 +6750,7 @@
       <c r="G195" s="12"/>
       <c r="H195" s="12"/>
     </row>
-    <row r="196" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="B196" s="12"/>
       <c r="C196" s="12"/>
@@ -6753,7 +6759,7 @@
       <c r="G196" s="12"/>
       <c r="H196" s="12"/>
     </row>
-    <row r="197" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="B197" s="12"/>
       <c r="C197" s="12"/>
@@ -6762,7 +6768,7 @@
       <c r="G197" s="12"/>
       <c r="H197" s="12"/>
     </row>
-    <row r="198" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12"/>
       <c r="B198" s="12"/>
       <c r="C198" s="12"/>
@@ -6771,7 +6777,7 @@
       <c r="G198" s="12"/>
       <c r="H198" s="12"/>
     </row>
-    <row r="199" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12"/>
       <c r="B199" s="12"/>
       <c r="C199" s="12"/>
@@ -6780,7 +6786,7 @@
       <c r="G199" s="12"/>
       <c r="H199" s="12"/>
     </row>
-    <row r="200" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12"/>
       <c r="B200" s="12"/>
       <c r="C200" s="12"/>
@@ -6789,7 +6795,7 @@
       <c r="G200" s="12"/>
       <c r="H200" s="12"/>
     </row>
-    <row r="201" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" s="12"/>
       <c r="C201" s="12"/>
@@ -6798,7 +6804,7 @@
       <c r="G201" s="12"/>
       <c r="H201" s="12"/>
     </row>
-    <row r="202" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" s="12"/>
       <c r="C202" s="12"/>
@@ -6807,7 +6813,7 @@
       <c r="G202" s="12"/>
       <c r="H202" s="12"/>
     </row>
-    <row r="203" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="B203" s="12"/>
       <c r="C203" s="12"/>
@@ -6816,7 +6822,7 @@
       <c r="G203" s="12"/>
       <c r="H203" s="12"/>
     </row>
-    <row r="204" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="B204" s="12"/>
       <c r="C204" s="12"/>
@@ -6825,7 +6831,7 @@
       <c r="G204" s="12"/>
       <c r="H204" s="12"/>
     </row>
-    <row r="205" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="B205" s="12"/>
       <c r="C205" s="12"/>
@@ -6834,7 +6840,7 @@
       <c r="G205" s="12"/>
       <c r="H205" s="12"/>
     </row>
-    <row r="206" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="B206" s="12"/>
       <c r="C206" s="12"/>
@@ -6843,7 +6849,7 @@
       <c r="G206" s="12"/>
       <c r="H206" s="12"/>
     </row>
-    <row r="207" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="B207" s="12"/>
       <c r="C207" s="12"/>
@@ -6852,7 +6858,7 @@
       <c r="G207" s="12"/>
       <c r="H207" s="12"/>
     </row>
-    <row r="208" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="B208" s="12"/>
       <c r="C208" s="12"/>
@@ -6861,7 +6867,7 @@
       <c r="G208" s="12"/>
       <c r="H208" s="12"/>
     </row>
-    <row r="209" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="B209" s="12"/>
       <c r="C209" s="12"/>
@@ -6870,7 +6876,7 @@
       <c r="G209" s="12"/>
       <c r="H209" s="12"/>
     </row>
-    <row r="210" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="B210" s="12"/>
       <c r="C210" s="12"/>
@@ -6879,7 +6885,7 @@
       <c r="G210" s="12"/>
       <c r="H210" s="12"/>
     </row>
-    <row r="211" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="B211" s="12"/>
       <c r="C211" s="12"/>
@@ -6888,7 +6894,7 @@
       <c r="G211" s="12"/>
       <c r="H211" s="12"/>
     </row>
-    <row r="212" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="B212" s="12"/>
       <c r="C212" s="12"/>
@@ -6897,7 +6903,7 @@
       <c r="G212" s="12"/>
       <c r="H212" s="12"/>
     </row>
-    <row r="213" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="B213" s="12"/>
       <c r="C213" s="12"/>
@@ -6906,7 +6912,7 @@
       <c r="G213" s="12"/>
       <c r="H213" s="12"/>
     </row>
-    <row r="214" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="B214" s="12"/>
       <c r="C214" s="12"/>
@@ -6915,7 +6921,7 @@
       <c r="G214" s="12"/>
       <c r="H214" s="12"/>
     </row>
-    <row r="215" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="B215" s="12"/>
       <c r="C215" s="12"/>
@@ -6924,7 +6930,7 @@
       <c r="G215" s="12"/>
       <c r="H215" s="12"/>
     </row>
-    <row r="216" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="B216" s="12"/>
       <c r="C216" s="12"/>
@@ -6933,7 +6939,7 @@
       <c r="G216" s="12"/>
       <c r="H216" s="12"/>
     </row>
-    <row r="217" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="B217" s="12"/>
       <c r="C217" s="12"/>
@@ -6942,7 +6948,7 @@
       <c r="G217" s="12"/>
       <c r="H217" s="12"/>
     </row>
-    <row r="218" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="B218" s="12"/>
       <c r="C218" s="12"/>
@@ -6951,7 +6957,7 @@
       <c r="G218" s="12"/>
       <c r="H218" s="12"/>
     </row>
-    <row r="219" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="12"/>
       <c r="B219" s="12"/>
       <c r="C219" s="12"/>
@@ -6960,7 +6966,7 @@
       <c r="G219" s="12"/>
       <c r="H219" s="12"/>
     </row>
-    <row r="220" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="12"/>
       <c r="B220" s="12"/>
       <c r="C220" s="12"/>
@@ -6969,7 +6975,7 @@
       <c r="G220" s="12"/>
       <c r="H220" s="12"/>
     </row>
-    <row r="221" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12"/>
       <c r="B221" s="12"/>
       <c r="C221" s="12"/>
@@ -6978,7 +6984,7 @@
       <c r="G221" s="12"/>
       <c r="H221" s="12"/>
     </row>
-    <row r="222" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="B222" s="12"/>
       <c r="C222" s="12"/>
@@ -6987,7 +6993,7 @@
       <c r="G222" s="12"/>
       <c r="H222" s="12"/>
     </row>
-    <row r="223" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="B223" s="12"/>
       <c r="C223" s="12"/>
@@ -6996,7 +7002,7 @@
       <c r="G223" s="12"/>
       <c r="H223" s="12"/>
     </row>
-    <row r="224" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="B224" s="12"/>
       <c r="C224" s="12"/>
@@ -7005,7 +7011,7 @@
       <c r="G224" s="12"/>
       <c r="H224" s="12"/>
     </row>
-    <row r="225" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="B225" s="12"/>
       <c r="C225" s="12"/>
@@ -7014,7 +7020,7 @@
       <c r="G225" s="12"/>
       <c r="H225" s="12"/>
     </row>
-    <row r="226" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="B226" s="12"/>
       <c r="C226" s="12"/>
@@ -7023,7 +7029,7 @@
       <c r="G226" s="12"/>
       <c r="H226" s="12"/>
     </row>
-    <row r="227" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12"/>
       <c r="B227" s="12"/>
       <c r="C227" s="12"/>
@@ -7032,7 +7038,7 @@
       <c r="G227" s="12"/>
       <c r="H227" s="12"/>
     </row>
-    <row r="228" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="12"/>
       <c r="B228" s="12"/>
       <c r="C228" s="12"/>
@@ -7041,7 +7047,7 @@
       <c r="G228" s="12"/>
       <c r="H228" s="12"/>
     </row>
-    <row r="229" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="12"/>
       <c r="B229" s="12"/>
       <c r="C229" s="12"/>
@@ -7050,7 +7056,7 @@
       <c r="G229" s="12"/>
       <c r="H229" s="12"/>
     </row>
-    <row r="230" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12"/>
       <c r="B230" s="12"/>
       <c r="C230" s="12"/>
@@ -7059,7 +7065,7 @@
       <c r="G230" s="12"/>
       <c r="H230" s="12"/>
     </row>
-    <row r="231" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="B231" s="12"/>
       <c r="C231" s="12"/>
@@ -7068,7 +7074,7 @@
       <c r="G231" s="12"/>
       <c r="H231" s="12"/>
     </row>
-    <row r="232" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" s="12"/>
       <c r="C232" s="12"/>
@@ -7077,7 +7083,7 @@
       <c r="G232" s="12"/>
       <c r="H232" s="12"/>
     </row>
-    <row r="233" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="B233" s="12"/>
       <c r="C233" s="12"/>
@@ -7086,7 +7092,7 @@
       <c r="G233" s="12"/>
       <c r="H233" s="12"/>
     </row>
-    <row r="234" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="B234" s="12"/>
       <c r="C234" s="12"/>
@@ -7095,7 +7101,7 @@
       <c r="G234" s="12"/>
       <c r="H234" s="12"/>
     </row>
-    <row r="235" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="B235" s="12"/>
       <c r="C235" s="12"/>
@@ -7104,7 +7110,7 @@
       <c r="G235" s="12"/>
       <c r="H235" s="12"/>
     </row>
-    <row r="236" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="B236" s="12"/>
       <c r="C236" s="12"/>
@@ -7113,7 +7119,7 @@
       <c r="G236" s="12"/>
       <c r="H236" s="12"/>
     </row>
-    <row r="237" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="B237" s="12"/>
       <c r="C237" s="12"/>
@@ -7122,7 +7128,7 @@
       <c r="G237" s="12"/>
       <c r="H237" s="12"/>
     </row>
-    <row r="238" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
       <c r="B238" s="12"/>
       <c r="C238" s="12"/>
@@ -7131,7 +7137,7 @@
       <c r="G238" s="12"/>
       <c r="H238" s="12"/>
     </row>
-    <row r="239" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
       <c r="B239" s="12"/>
       <c r="C239" s="12"/>
@@ -7140,7 +7146,7 @@
       <c r="G239" s="12"/>
       <c r="H239" s="12"/>
     </row>
-    <row r="240" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="12"/>
       <c r="B240" s="12"/>
       <c r="C240" s="12"/>
@@ -7149,7 +7155,7 @@
       <c r="G240" s="12"/>
       <c r="H240" s="12"/>
     </row>
-    <row r="241" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="B241" s="12"/>
       <c r="C241" s="12"/>
@@ -7158,7 +7164,7 @@
       <c r="G241" s="12"/>
       <c r="H241" s="12"/>
     </row>
-    <row r="242" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="12"/>
       <c r="B242" s="12"/>
       <c r="C242" s="12"/>
@@ -7167,7 +7173,7 @@
       <c r="G242" s="12"/>
       <c r="H242" s="12"/>
     </row>
-    <row r="243" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="12"/>
       <c r="B243" s="12"/>
       <c r="C243" s="12"/>
@@ -7176,7 +7182,7 @@
       <c r="G243" s="12"/>
       <c r="H243" s="12"/>
     </row>
-    <row r="244" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="12"/>
       <c r="B244" s="12"/>
       <c r="C244" s="12"/>
@@ -7185,7 +7191,7 @@
       <c r="G244" s="12"/>
       <c r="H244" s="12"/>
     </row>
-    <row r="245" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="12"/>
       <c r="B245" s="12"/>
       <c r="C245" s="12"/>
@@ -7194,7 +7200,7 @@
       <c r="G245" s="12"/>
       <c r="H245" s="12"/>
     </row>
-    <row r="246" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="12"/>
       <c r="B246" s="12"/>
       <c r="C246" s="12"/>
@@ -7203,7 +7209,7 @@
       <c r="G246" s="12"/>
       <c r="H246" s="12"/>
     </row>
-    <row r="247" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="12"/>
       <c r="B247" s="12"/>
       <c r="C247" s="12"/>
@@ -7212,7 +7218,7 @@
       <c r="G247" s="12"/>
       <c r="H247" s="12"/>
     </row>
-    <row r="248" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" s="12"/>
       <c r="C248" s="12"/>
@@ -7221,7 +7227,7 @@
       <c r="G248" s="12"/>
       <c r="H248" s="12"/>
     </row>
-    <row r="249" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="B249" s="12"/>
       <c r="C249" s="12"/>
@@ -7230,7 +7236,7 @@
       <c r="G249" s="12"/>
       <c r="H249" s="12"/>
     </row>
-    <row r="250" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" s="12"/>
       <c r="C250" s="12"/>
@@ -7239,7 +7245,7 @@
       <c r="G250" s="12"/>
       <c r="H250" s="12"/>
     </row>
-    <row r="251" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" s="12"/>
       <c r="C251" s="12"/>
@@ -7248,7 +7254,7 @@
       <c r="G251" s="12"/>
       <c r="H251" s="12"/>
     </row>
-    <row r="252" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" s="12"/>
       <c r="C252" s="12"/>
@@ -7257,7 +7263,7 @@
       <c r="G252" s="12"/>
       <c r="H252" s="12"/>
     </row>
-    <row r="253" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="B253" s="12"/>
       <c r="C253" s="12"/>
@@ -7266,7 +7272,7 @@
       <c r="G253" s="12"/>
       <c r="H253" s="12"/>
     </row>
-    <row r="254" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" s="12"/>
       <c r="C254" s="12"/>
@@ -7275,7 +7281,7 @@
       <c r="G254" s="12"/>
       <c r="H254" s="12"/>
     </row>
-    <row r="255" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="B255" s="12"/>
       <c r="C255" s="12"/>
@@ -7284,7 +7290,7 @@
       <c r="G255" s="12"/>
       <c r="H255" s="12"/>
     </row>
-    <row r="256" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" s="12"/>
       <c r="C256" s="12"/>
@@ -7293,7 +7299,7 @@
       <c r="G256" s="12"/>
       <c r="H256" s="12"/>
     </row>
-    <row r="257" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" s="12"/>
       <c r="C257" s="12"/>
@@ -7302,7 +7308,7 @@
       <c r="G257" s="12"/>
       <c r="H257" s="12"/>
     </row>
-    <row r="258" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" s="12"/>
       <c r="C258" s="12"/>
@@ -7311,7 +7317,7 @@
       <c r="G258" s="12"/>
       <c r="H258" s="12"/>
     </row>
-    <row r="259" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" s="12"/>
       <c r="C259" s="12"/>
@@ -7320,7 +7326,7 @@
       <c r="G259" s="12"/>
       <c r="H259" s="12"/>
     </row>
-    <row r="260" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" s="12"/>
       <c r="C260" s="12"/>
@@ -7329,7 +7335,7 @@
       <c r="G260" s="12"/>
       <c r="H260" s="12"/>
     </row>
-    <row r="261" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="12"/>
       <c r="B261" s="12"/>
       <c r="C261" s="12"/>
@@ -7338,7 +7344,7 @@
       <c r="G261" s="12"/>
       <c r="H261" s="12"/>
     </row>
-    <row r="262" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="12"/>
       <c r="B262" s="12"/>
       <c r="C262" s="12"/>
@@ -7347,7 +7353,7 @@
       <c r="G262" s="12"/>
       <c r="H262" s="12"/>
     </row>
-    <row r="263" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="12"/>
       <c r="B263" s="12"/>
       <c r="C263" s="12"/>
@@ -7356,7 +7362,7 @@
       <c r="G263" s="12"/>
       <c r="H263" s="12"/>
     </row>
-    <row r="264" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="12"/>
       <c r="B264" s="12"/>
       <c r="C264" s="12"/>
@@ -7365,7 +7371,7 @@
       <c r="G264" s="12"/>
       <c r="H264" s="12"/>
     </row>
-    <row r="265" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="12"/>
       <c r="B265" s="12"/>
       <c r="C265" s="12"/>
@@ -7374,7 +7380,7 @@
       <c r="G265" s="12"/>
       <c r="H265" s="12"/>
     </row>
-    <row r="266" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="12"/>
       <c r="B266" s="12"/>
       <c r="C266" s="12"/>
@@ -7383,7 +7389,7 @@
       <c r="G266" s="12"/>
       <c r="H266" s="12"/>
     </row>
-    <row r="267" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="12"/>
       <c r="B267" s="12"/>
       <c r="C267" s="12"/>
@@ -7392,7 +7398,7 @@
       <c r="G267" s="12"/>
       <c r="H267" s="12"/>
     </row>
-    <row r="268" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="12"/>
       <c r="B268" s="12"/>
       <c r="C268" s="12"/>
@@ -7401,7 +7407,7 @@
       <c r="G268" s="12"/>
       <c r="H268" s="12"/>
     </row>
-    <row r="269" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="12"/>
       <c r="B269" s="12"/>
       <c r="C269" s="12"/>
@@ -7410,7 +7416,7 @@
       <c r="G269" s="12"/>
       <c r="H269" s="12"/>
     </row>
-    <row r="270" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="12"/>
       <c r="B270" s="12"/>
       <c r="C270" s="12"/>
@@ -7419,7 +7425,7 @@
       <c r="G270" s="12"/>
       <c r="H270" s="12"/>
     </row>
-    <row r="271" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="12"/>
       <c r="B271" s="12"/>
       <c r="C271" s="12"/>
@@ -7428,7 +7434,7 @@
       <c r="G271" s="12"/>
       <c r="H271" s="12"/>
     </row>
-    <row r="272" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="12"/>
       <c r="B272" s="12"/>
       <c r="C272" s="12"/>
@@ -7437,7 +7443,7 @@
       <c r="G272" s="12"/>
       <c r="H272" s="12"/>
     </row>
-    <row r="273" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="12"/>
       <c r="B273" s="12"/>
       <c r="C273" s="12"/>
@@ -7446,7 +7452,7 @@
       <c r="G273" s="12"/>
       <c r="H273" s="12"/>
     </row>
-    <row r="274" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="12"/>
       <c r="B274" s="12"/>
       <c r="C274" s="12"/>
@@ -7455,7 +7461,7 @@
       <c r="G274" s="12"/>
       <c r="H274" s="12"/>
     </row>
-    <row r="275" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="12"/>
       <c r="B275" s="12"/>
       <c r="C275" s="12"/>
@@ -7464,7 +7470,7 @@
       <c r="G275" s="12"/>
       <c r="H275" s="12"/>
     </row>
-    <row r="276" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="12"/>
       <c r="B276" s="12"/>
       <c r="C276" s="12"/>
@@ -7473,7 +7479,7 @@
       <c r="G276" s="12"/>
       <c r="H276" s="12"/>
     </row>
-    <row r="277" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="12"/>
       <c r="B277" s="12"/>
       <c r="C277" s="12"/>
@@ -7482,7 +7488,7 @@
       <c r="G277" s="12"/>
       <c r="H277" s="12"/>
     </row>
-    <row r="278" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="12"/>
       <c r="B278" s="12"/>
       <c r="C278" s="12"/>
@@ -8331,33 +8337,33 @@
   <dimension ref="A1:AF984"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.08984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.54296875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.6328125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="8.90625" style="6"/>
-    <col min="13" max="13" width="9.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.36328125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="6"/>
+    <col min="13" max="13" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" style="6" customWidth="1"/>
     <col min="15" max="15" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.90625" style="6"/>
-    <col min="17" max="28" width="7.6328125" style="6" customWidth="1"/>
-    <col min="29" max="16384" width="12.6328125" style="6"/>
+    <col min="16" max="16" width="8.88671875" style="6"/>
+    <col min="17" max="28" width="7.6640625" style="6" customWidth="1"/>
+    <col min="29" max="16384" width="12.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>134</v>
       </c>
@@ -8422,7 +8428,7 @@
       <c r="AB1" s="9"/>
       <c r="AC1" s="9"/>
     </row>
-    <row r="2" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>597</v>
       </c>
@@ -8445,7 +8451,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>598</v>
       </c>
@@ -8468,7 +8474,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>595</v>
       </c>
@@ -8491,7 +8497,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>147</v>
       </c>
@@ -8508,7 +8514,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
         <v>149</v>
       </c>
@@ -8525,7 +8531,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
         <v>151</v>
       </c>
@@ -8542,7 +8548,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
         <v>154</v>
       </c>
@@ -8559,7 +8565,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="9" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
         <v>156</v>
       </c>
@@ -8576,7 +8582,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
         <v>158</v>
       </c>
@@ -8593,7 +8599,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
         <v>160</v>
       </c>
@@ -8610,7 +8616,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>162</v>
       </c>
@@ -8627,7 +8633,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>164</v>
       </c>
@@ -8644,7 +8650,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>581</v>
       </c>
@@ -8678,8 +8684,13 @@
       <c r="AE14" s="12"/>
       <c r="AF14" s="12"/>
     </row>
-    <row r="15" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A15"/>
+    <row r="15" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>660</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>659</v>
+      </c>
       <c r="C15" s="6" t="s">
         <v>166</v>
       </c>
@@ -8696,7 +8707,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
         <v>169</v>
       </c>
@@ -8713,7 +8724,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C17" s="6" t="s">
         <v>599</v>
       </c>
@@ -8730,7 +8741,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C18" s="6" t="s">
         <v>600</v>
       </c>
@@ -8828,7 +8839,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C22" s="6" t="s">
         <v>171</v>
       </c>
@@ -8857,7 +8868,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>176</v>
       </c>
@@ -8898,7 +8909,7 @@
       <c r="AA23" s="9"/>
       <c r="AB23" s="9"/>
     </row>
-    <row r="24" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
         <v>178</v>
       </c>
@@ -8940,7 +8951,7 @@
       <c r="AA24" s="9"/>
       <c r="AB24" s="9"/>
     </row>
-    <row r="25" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
         <v>180</v>
       </c>
@@ -8969,7 +8980,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C26" s="6" t="s">
         <v>182</v>
       </c>
@@ -9216,9 +9227,6 @@
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35"/>
-      <c r="B35" s="6" t="s">
-        <v>175</v>
-      </c>
       <c r="C35" s="7" t="s">
         <v>639</v>
       </c>
@@ -10319,9 +10327,9 @@
         <v>207</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>654</v>
+    <row r="77" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="19" t="s">
+        <v>658</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>437</v>
@@ -10330,10 +10338,10 @@
         <v>653</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>121</v>
@@ -10366,18 +10374,18 @@
       <c r="AA77" s="13"/>
       <c r="AB77" s="13"/>
     </row>
-    <row r="78" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>121</v>
@@ -10683,7 +10691,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C92" s="6" t="s">
         <v>283</v>
       </c>
@@ -10724,7 +10732,7 @@
       <c r="AA92" s="13"/>
       <c r="AB92" s="13"/>
     </row>
-    <row r="93" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="6" t="s">
         <v>286</v>
       </c>
@@ -10765,7 +10773,7 @@
       <c r="AA93" s="13"/>
       <c r="AB93" s="13"/>
     </row>
-    <row r="94" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C94" s="6" t="s">
         <v>288</v>
       </c>
@@ -10797,7 +10805,7 @@
       <c r="AA94" s="13"/>
       <c r="AB94" s="13"/>
     </row>
-    <row r="95" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="6" t="s">
         <v>290</v>
       </c>
@@ -10838,7 +10846,7 @@
       <c r="AA95" s="13"/>
       <c r="AB95" s="13"/>
     </row>
-    <row r="96" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="6" t="s">
         <v>292</v>
       </c>
@@ -10879,7 +10887,7 @@
       <c r="AA96" s="13"/>
       <c r="AB96" s="13"/>
     </row>
-    <row r="97" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C97" s="6" t="s">
         <v>294</v>
       </c>
@@ -10920,7 +10928,7 @@
       <c r="AA97" s="13"/>
       <c r="AB97" s="13"/>
     </row>
-    <row r="98" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C98" s="6" t="s">
         <v>296</v>
       </c>
@@ -10952,7 +10960,7 @@
       <c r="AA98" s="13"/>
       <c r="AB98" s="13"/>
     </row>
-    <row r="99" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C99" s="6" t="s">
         <v>298</v>
       </c>
@@ -10993,7 +11001,7 @@
       <c r="AA99" s="13"/>
       <c r="AB99" s="13"/>
     </row>
-    <row r="100" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C100" s="6" t="s">
         <v>300</v>
       </c>
@@ -11034,7 +11042,7 @@
       <c r="AA100" s="13"/>
       <c r="AB100" s="13"/>
     </row>
-    <row r="101" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C101" s="6" t="s">
         <v>302</v>
       </c>
@@ -11075,7 +11083,7 @@
       <c r="AA101" s="13"/>
       <c r="AB101" s="13"/>
     </row>
-    <row r="102" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C102" s="6" t="s">
         <v>304</v>
       </c>
@@ -11116,7 +11124,7 @@
       <c r="AA102" s="13"/>
       <c r="AB102" s="13"/>
     </row>
-    <row r="103" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="6" t="s">
         <v>306</v>
       </c>
@@ -11151,7 +11159,7 @@
       <c r="AA103" s="13"/>
       <c r="AB103" s="13"/>
     </row>
-    <row r="104" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C104" s="6" t="s">
         <v>308</v>
       </c>
@@ -11192,7 +11200,7 @@
       <c r="AA104" s="13"/>
       <c r="AB104" s="13"/>
     </row>
-    <row r="105" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C105" s="6" t="s">
         <v>310</v>
       </c>
@@ -11233,7 +11241,7 @@
       <c r="AA105" s="13"/>
       <c r="AB105" s="13"/>
     </row>
-    <row r="106" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C106" s="6" t="s">
         <v>312</v>
       </c>
@@ -11274,7 +11282,7 @@
       <c r="AA106" s="13"/>
       <c r="AB106" s="13"/>
     </row>
-    <row r="107" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C107" s="6" t="s">
         <v>314</v>
       </c>
@@ -11312,7 +11320,7 @@
       <c r="AA107" s="13"/>
       <c r="AB107" s="13"/>
     </row>
-    <row r="108" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C108" s="6" t="s">
         <v>316</v>
       </c>
@@ -11353,7 +11361,7 @@
       <c r="AA108" s="13"/>
       <c r="AB108" s="13"/>
     </row>
-    <row r="109" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C109" s="6" t="s">
         <v>319</v>
       </c>
@@ -11394,7 +11402,7 @@
       <c r="AA109" s="13"/>
       <c r="AB109" s="13"/>
     </row>
-    <row r="110" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C110" s="6" t="s">
         <v>321</v>
       </c>
@@ -11435,7 +11443,7 @@
       <c r="AA110" s="13"/>
       <c r="AB110" s="13"/>
     </row>
-    <row r="111" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C111" s="6" t="s">
         <v>323</v>
       </c>
@@ -11476,7 +11484,7 @@
       <c r="AA111" s="13"/>
       <c r="AB111" s="13"/>
     </row>
-    <row r="112" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C112" s="6" t="s">
         <v>325</v>
       </c>
@@ -11517,7 +11525,7 @@
       <c r="AA112" s="13"/>
       <c r="AB112" s="13"/>
     </row>
-    <row r="113" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C113" s="6" t="s">
         <v>327</v>
       </c>
@@ -11558,7 +11566,7 @@
       <c r="AA113" s="13"/>
       <c r="AB113" s="13"/>
     </row>
-    <row r="114" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C114" s="6" t="s">
         <v>329</v>
       </c>
@@ -11599,7 +11607,7 @@
       <c r="AA114" s="13"/>
       <c r="AB114" s="13"/>
     </row>
-    <row r="115" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C115" s="6" t="s">
         <v>331</v>
       </c>
@@ -11640,7 +11648,7 @@
       <c r="AA115" s="13"/>
       <c r="AB115" s="13"/>
     </row>
-    <row r="116" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C116" s="6" t="s">
         <v>333</v>
       </c>
@@ -11681,7 +11689,7 @@
       <c r="AA116" s="13"/>
       <c r="AB116" s="13"/>
     </row>
-    <row r="117" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="6" t="s">
         <v>335</v>
       </c>
@@ -11722,7 +11730,7 @@
       <c r="AA117" s="13"/>
       <c r="AB117" s="13"/>
     </row>
-    <row r="118" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="6" t="s">
         <v>337</v>
       </c>
@@ -11763,7 +11771,7 @@
       <c r="AA118" s="13"/>
       <c r="AB118" s="13"/>
     </row>
-    <row r="119" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C119" s="6" t="s">
         <v>339</v>
       </c>
@@ -11804,7 +11812,7 @@
       <c r="AA119" s="13"/>
       <c r="AB119" s="13"/>
     </row>
-    <row r="120" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C120" s="6" t="s">
         <v>341</v>
       </c>
@@ -11845,7 +11853,7 @@
       <c r="AA120" s="13"/>
       <c r="AB120" s="13"/>
     </row>
-    <row r="121" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C121" s="6" t="s">
         <v>343</v>
       </c>
@@ -11886,7 +11894,7 @@
       <c r="AA121" s="13"/>
       <c r="AB121" s="13"/>
     </row>
-    <row r="122" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C122" s="6" t="s">
         <v>345</v>
       </c>
@@ -11918,7 +11926,7 @@
       <c r="AA122" s="13"/>
       <c r="AB122" s="13"/>
     </row>
-    <row r="123" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C123" s="6" t="s">
         <v>347</v>
       </c>
@@ -11950,7 +11958,7 @@
       <c r="AA123" s="13"/>
       <c r="AB123" s="13"/>
     </row>
-    <row r="124" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C124" s="6" t="s">
         <v>349</v>
       </c>
@@ -11985,7 +11993,7 @@
       <c r="AA124" s="13"/>
       <c r="AB124" s="13"/>
     </row>
-    <row r="125" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C125" s="6" t="s">
         <v>351</v>
       </c>
@@ -12026,7 +12034,7 @@
       <c r="AA125" s="13"/>
       <c r="AB125" s="13"/>
     </row>
-    <row r="126" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C126" s="6" t="s">
         <v>353</v>
       </c>
@@ -12067,7 +12075,7 @@
       <c r="AA126" s="13"/>
       <c r="AB126" s="13"/>
     </row>
-    <row r="127" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C127" s="6" t="s">
         <v>356</v>
       </c>
@@ -12105,7 +12113,7 @@
       <c r="AA127" s="13"/>
       <c r="AB127" s="13"/>
     </row>
-    <row r="128" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="6" t="s">
         <v>358</v>
       </c>
@@ -13073,14 +13081,14 @@
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" customWidth="1"/>
+    <col min="1" max="2" width="11.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>583</v>
       </c>
@@ -13094,7 +13102,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>175</v>
       </c>
@@ -13105,7 +13113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>175</v>
       </c>
@@ -13116,7 +13124,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>175</v>
       </c>
@@ -13127,7 +13135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>175</v>
       </c>
@@ -13138,7 +13146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>175</v>
       </c>
@@ -13149,7 +13157,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>175</v>
       </c>
@@ -13160,7 +13168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>175</v>
       </c>
@@ -13171,7 +13179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>101</v>
       </c>
@@ -13182,7 +13190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>101</v>
       </c>
@@ -13193,7 +13201,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>101</v>
       </c>
@@ -13204,7 +13212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>230</v>
       </c>
@@ -13215,7 +13223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>230</v>
       </c>
@@ -13226,7 +13234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>230</v>
       </c>
@@ -13237,7 +13245,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>522</v>
       </c>
@@ -13251,7 +13259,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>421</v>
       </c>
@@ -13262,7 +13270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>421</v>
       </c>
@@ -13273,7 +13281,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>421</v>
       </c>
@@ -13284,7 +13292,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>361</v>
       </c>
@@ -13295,7 +13303,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>511</v>
       </c>
@@ -13306,7 +13314,7 @@
         <v>0.30480000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>502</v>
       </c>
@@ -13317,7 +13325,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>402</v>
       </c>
@@ -13328,7 +13336,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>402</v>
       </c>
@@ -13339,7 +13347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>402</v>
       </c>
@@ -13350,7 +13358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>402</v>
       </c>
@@ -13361,7 +13369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>402</v>
       </c>
@@ -13372,7 +13380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>402</v>
       </c>
@@ -13383,7 +13391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>402</v>
       </c>
@@ -13394,7 +13402,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>385</v>
       </c>
@@ -13405,7 +13413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>385</v>
       </c>
@@ -13416,7 +13424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>385</v>
       </c>
@@ -13427,7 +13435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>385</v>
       </c>
@@ -13438,7 +13446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>387</v>
       </c>
@@ -13449,7 +13457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>503</v>
       </c>
@@ -13460,7 +13468,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>438</v>
       </c>
@@ -13471,7 +13479,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>438</v>
       </c>
@@ -13482,7 +13490,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>438</v>
       </c>
@@ -13493,7 +13501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>422</v>
       </c>
@@ -13504,7 +13512,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>420</v>
       </c>
@@ -13515,7 +13523,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>420</v>
       </c>
@@ -13526,7 +13534,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>420</v>
       </c>
@@ -13537,7 +13545,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>420</v>
       </c>
@@ -13548,7 +13556,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>403</v>
       </c>
@@ -13559,7 +13567,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>403</v>
       </c>
@@ -13570,7 +13578,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>403</v>
       </c>
@@ -13581,7 +13589,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>403</v>
       </c>
@@ -13592,7 +13600,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>404</v>
       </c>
@@ -13603,7 +13611,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>404</v>
       </c>
@@ -13614,7 +13622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>451</v>
       </c>
@@ -13625,7 +13633,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>451</v>
       </c>
@@ -13636,7 +13644,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>451</v>
       </c>
@@ -13647,7 +13655,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>439</v>
       </c>
@@ -13658,7 +13666,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>439</v>
       </c>
@@ -13669,7 +13677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>510</v>
       </c>
@@ -13680,7 +13688,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>41</v>
       </c>
@@ -13691,7 +13699,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>41</v>
       </c>
@@ -13702,7 +13710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>41</v>
       </c>
@@ -13713,7 +13721,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>584</v>
       </c>
@@ -13724,7 +13732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>233</v>
       </c>
@@ -13735,7 +13743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>233</v>
       </c>
@@ -13746,7 +13754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>233</v>
       </c>
@@ -13757,7 +13765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>500</v>
       </c>
@@ -13768,7 +13776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>500</v>
       </c>
@@ -13779,7 +13787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>437</v>
       </c>
@@ -13790,7 +13798,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>437</v>
       </c>
@@ -13801,7 +13809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>437</v>
       </c>
@@ -13812,7 +13820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>437</v>
       </c>
@@ -13823,7 +13831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>437</v>
       </c>
@@ -13834,7 +13842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>437</v>
       </c>
@@ -13845,7 +13853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>437</v>
       </c>
@@ -13856,7 +13864,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>507</v>
       </c>
@@ -13867,7 +13875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>419</v>
       </c>
@@ -13878,7 +13886,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>419</v>
       </c>
@@ -13889,7 +13897,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>419</v>
       </c>
@@ -13900,7 +13908,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>419</v>
       </c>
@@ -13911,7 +13919,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>419</v>
       </c>
@@ -13922,7 +13930,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>419</v>
       </c>
@@ -13933,7 +13941,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>419</v>
       </c>
@@ -13944,7 +13952,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>509</v>
       </c>
@@ -13955,7 +13963,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>44</v>
       </c>
@@ -13966,7 +13974,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>44</v>
       </c>
@@ -13977,7 +13985,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>44</v>
       </c>
@@ -13988,7 +13996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>462</v>
       </c>
@@ -13999,7 +14007,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>462</v>
       </c>
@@ -14010,7 +14018,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>462</v>
       </c>
@@ -14021,7 +14029,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>462</v>
       </c>
@@ -14032,7 +14040,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>452</v>
       </c>
@@ -14043,7 +14051,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>452</v>
       </c>
@@ -14172,13 +14180,13 @@
       <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
-    <col min="2" max="26" width="7.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="26" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>362</v>
       </c>
@@ -14258,7 +14266,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>383</v>
       </c>
@@ -14338,7 +14346,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>401</v>
       </c>
@@ -14412,7 +14420,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>417</v>
       </c>
@@ -14480,7 +14488,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -14539,7 +14547,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>448</v>
       </c>
@@ -14592,7 +14600,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>460</v>
       </c>
@@ -14639,7 +14647,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>471</v>
       </c>
@@ -14677,7 +14685,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>480</v>
       </c>
@@ -14712,7 +14720,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>487</v>
       </c>
@@ -14738,7 +14746,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>491</v>
       </c>
@@ -14755,7 +14763,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>494</v>
       </c>
@@ -14772,7 +14780,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="M13" t="s">
         <v>120</v>
       </c>
@@ -14783,12 +14791,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="T14" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="S15" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>